<commit_message>
reports and everything along with it
</commit_message>
<xml_diff>
--- a/number-changes/number_changes.xlsx
+++ b/number-changes/number_changes.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="CHW" sheetId="1" r:id="rId4"/>
-    <sheet name="PS" sheetId="2" r:id="rId5"/>
+    <sheet name="CHW Other Changes" sheetId="2" r:id="rId5"/>
+    <sheet name="PS" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
   <si>
     <t>district_label</t>
   </si>
@@ -36,6 +37,9 @@
     <t>new_payment_number</t>
   </si>
   <si>
+    <t>note</t>
+  </si>
+  <si>
     <t>Tonkolili</t>
   </si>
   <si>
@@ -51,6 +55,9 @@
     <t>Sesay</t>
   </si>
   <si>
+    <t>request</t>
+  </si>
+  <si>
     <t>Manewo</t>
   </si>
   <si>
@@ -144,6 +151,192 @@
     <t>Sheku</t>
   </si>
   <si>
+    <t>Simbaru</t>
+  </si>
+  <si>
+    <t>Gbamgbina</t>
+  </si>
+  <si>
+    <t>Morisa</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Lower Bambara</t>
+  </si>
+  <si>
+    <t>Kornia Kpindem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vandi </t>
+  </si>
+  <si>
+    <t>Musa</t>
+  </si>
+  <si>
+    <t>Naiwa</t>
+  </si>
+  <si>
+    <t>Gorahun</t>
+  </si>
+  <si>
+    <t>Muctarr</t>
+  </si>
+  <si>
+    <t>Duwai</t>
+  </si>
+  <si>
+    <t>request -not in Survey CTO</t>
+  </si>
+  <si>
+    <t>Mathamp</t>
+  </si>
+  <si>
+    <t>Gbla</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Western Area</t>
+  </si>
+  <si>
+    <t>A-F</t>
+  </si>
+  <si>
+    <t>Charlotte CHP</t>
+  </si>
+  <si>
+    <t>RAYMOND PRINCE</t>
+  </si>
+  <si>
+    <t>HARDING</t>
+  </si>
+  <si>
+    <t>23276430975</t>
+  </si>
+  <si>
+    <t>duplicated</t>
+  </si>
+  <si>
+    <t>Biriwa</t>
+  </si>
+  <si>
+    <t>Kamabai</t>
+  </si>
+  <si>
+    <t>MOHAMED</t>
+  </si>
+  <si>
+    <t>KOROMA</t>
+  </si>
+  <si>
+    <t>23278102094</t>
+  </si>
+  <si>
+    <t>Kunike Sanda</t>
+  </si>
+  <si>
+    <t>Matholley</t>
+  </si>
+  <si>
+    <t>JOSEPH R</t>
+  </si>
+  <si>
+    <t>23278112752</t>
+  </si>
+  <si>
+    <t>23276495561</t>
+  </si>
+  <si>
+    <t>Kambia</t>
+  </si>
+  <si>
+    <t>Mambolo</t>
+  </si>
+  <si>
+    <t>Mayakie</t>
+  </si>
+  <si>
+    <t>LAMIN J</t>
+  </si>
+  <si>
+    <t>KARGBO</t>
+  </si>
+  <si>
+    <t>23278409554</t>
+  </si>
+  <si>
+    <t>Lowoma</t>
+  </si>
+  <si>
+    <t>HAWA</t>
+  </si>
+  <si>
+    <t>BRIMA</t>
+  </si>
+  <si>
+    <t>23279303204</t>
+  </si>
+  <si>
+    <t>23279194260</t>
+  </si>
+  <si>
+    <t>Kalainkay</t>
+  </si>
+  <si>
+    <t>Fatmata</t>
+  </si>
+  <si>
+    <t>z08_2 africell</t>
+  </si>
+  <si>
+    <t>Tane</t>
+  </si>
+  <si>
+    <t>Matotoka</t>
+  </si>
+  <si>
+    <t>OSMAN M</t>
+  </si>
+  <si>
+    <t>THOLLEY</t>
+  </si>
+  <si>
+    <t>IBRAHIM F</t>
+  </si>
+  <si>
+    <t>SESAY</t>
+  </si>
+  <si>
+    <t>Bumpe Ngao</t>
+  </si>
+  <si>
+    <t>Bumpe CHC</t>
+  </si>
+  <si>
+    <t>MOMODU</t>
+  </si>
+  <si>
+    <t>SMART</t>
+  </si>
+  <si>
+    <t>Tunkia</t>
+  </si>
+  <si>
+    <t>Geigbwema</t>
+  </si>
+  <si>
+    <t>JENNEH</t>
+  </si>
+  <si>
+    <t>SARGIE</t>
+  </si>
+  <si>
+    <t>z08_2 invalid</t>
+  </si>
+  <si>
     <t>Bombali Sebora</t>
   </si>
   <si>
@@ -154,6 +347,18 @@
   </si>
   <si>
     <t>Conteh</t>
+  </si>
+  <si>
+    <t>Dodo</t>
+  </si>
+  <si>
+    <t>Kundorma</t>
+  </si>
+  <si>
+    <t>Christopher B</t>
+  </si>
+  <si>
+    <t>Amara</t>
   </si>
 </sst>
 </file>
@@ -191,7 +396,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,12 +411,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -221,14 +450,51 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
@@ -236,136 +502,46 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -375,7 +551,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -385,58 +561,88 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -457,9 +663,14 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff00f900"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="fffefb00"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1524,7 +1735,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1535,12 +1746,13 @@
     <col min="3" max="3" width="14.8516" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.67188" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1719" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.6719" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.65" customHeight="1">
+    <row r="1" ht="15.6" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1562,22 +1774,25 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
+    </row>
+    <row r="2" ht="13.7" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>8</v>
+      </c>
       <c r="B2" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="C2" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="D2" t="s" s="4">
         <v>11</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>12</v>
       </c>
       <c r="F2" s="5">
         <v>23278408530</v>
@@ -1585,212 +1800,346 @@
       <c r="G2" s="5">
         <v>23279040385</v>
       </c>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s" s="3">
+      <c r="H2" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" ht="13.7" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="B3" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5">
+        <v>23278415586</v>
+      </c>
+      <c r="G3" s="5">
+        <v>23276131417</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="13.7" customHeight="1">
+      <c r="A4" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="4">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="F4" s="5">
+        <v>23278114298</v>
+      </c>
+      <c r="G4" s="5">
+        <v>23278111587</v>
+      </c>
+      <c r="H4" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7">
-        <v>23278415586</v>
-      </c>
-      <c r="G3" s="7">
-        <v>23276131417</v>
-      </c>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s" s="6">
+    </row>
+    <row r="5" ht="13.7" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s" s="4">
+        <v>24</v>
+      </c>
+      <c r="F5" s="9">
+        <v>23276631349</v>
+      </c>
+      <c r="G5" s="5">
+        <v>23276612301</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="13.7" customHeight="1">
+      <c r="A6" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="F6" s="5">
+        <v>23279290576</v>
+      </c>
+      <c r="G6" s="5">
+        <v>23278860269</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" ht="13.7" customHeight="1">
+      <c r="A7" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s" s="4">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5">
+        <v>23276380941</v>
+      </c>
+      <c r="G7" s="5">
+        <v>23278836029</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="13.7" customHeight="1">
+      <c r="A8" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s" s="4">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5">
+        <v>23279337425</v>
+      </c>
+      <c r="G8" s="5">
+        <v>23278837207</v>
+      </c>
+      <c r="H8" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="13.7" customHeight="1">
+      <c r="A9" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s" s="4">
+        <v>34</v>
+      </c>
+      <c r="F9" s="5">
+        <v>23279336841</v>
+      </c>
+      <c r="G9" s="5">
+        <v>23278836705</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="13.7" customHeight="1">
+      <c r="A10" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5">
+        <v>23276201816</v>
+      </c>
+      <c r="G10" s="5">
+        <v>23276163991</v>
+      </c>
+      <c r="H10" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" ht="14.65" customHeight="1">
+      <c r="A11" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="F11" s="11">
+        <v>23278301366</v>
+      </c>
+      <c r="G11" s="11">
+        <v>23278804642</v>
+      </c>
+      <c r="H11" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" ht="15.2" customHeight="1">
+      <c r="A12" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s" s="10">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s" s="10">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="F12" s="11">
+        <v>23278316330</v>
+      </c>
+      <c r="G12" s="11">
+        <v>23278762917</v>
+      </c>
+      <c r="H12" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" ht="15.2" customHeight="1">
+      <c r="A13" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s" s="10">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s" s="10">
+        <v>52</v>
+      </c>
+      <c r="F13" s="11">
+        <v>23279303649</v>
+      </c>
+      <c r="G13" s="11">
+        <v>23279506988</v>
+      </c>
+      <c r="H13" t="s" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" ht="15.2" customHeight="1">
+      <c r="A14" t="s" s="12">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s" s="12">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="13">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s" s="12">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s" s="12">
+        <v>56</v>
+      </c>
+      <c r="F14" s="14">
+        <v>23276577690</v>
+      </c>
+      <c r="G14" s="14">
+        <v>23276141823</v>
+      </c>
+      <c r="H14" t="s" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" ht="15.2" customHeight="1">
+      <c r="A15" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s" s="12">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="F4" s="9">
-        <v>23278114298</v>
-      </c>
-      <c r="G4" s="7">
-        <v>23278111587</v>
-      </c>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s" s="12">
-        <v>22</v>
-      </c>
-      <c r="F5" s="13">
-        <v>23276631349</v>
-      </c>
-      <c r="G5" s="7">
-        <v>23276612301</v>
-      </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="F6" s="14">
-        <v>23279290576</v>
-      </c>
-      <c r="G6" s="7">
-        <v>23278860269</v>
-      </c>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="F7" s="7">
-        <v>23279290576</v>
-      </c>
-      <c r="G7" s="7">
-        <v>23278836029</v>
-      </c>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="F8" s="7">
-        <v>23279337425</v>
-      </c>
-      <c r="G8" s="7">
-        <v>23278837207</v>
-      </c>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="F9" s="7">
-        <v>23279336841</v>
-      </c>
-      <c r="G9" s="7">
-        <v>23278836705</v>
-      </c>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="F10" s="7">
-        <v>23276201816</v>
-      </c>
-      <c r="G10" s="7">
-        <v>23276163991</v>
-      </c>
-    </row>
-    <row r="11" ht="14.7" customHeight="1">
-      <c r="A11" t="s" s="15">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s" s="15">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s" s="15">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s" s="15">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s" s="15">
-        <v>42</v>
-      </c>
-      <c r="F11" s="16">
-        <v>23278301366</v>
-      </c>
-      <c r="G11" s="16">
-        <v>23278804642</v>
+      <c r="E15" t="s" s="12">
+        <v>59</v>
+      </c>
+      <c r="F15" s="14">
+        <v>23276642381</v>
+      </c>
+      <c r="G15" s="14">
+        <v>23276390787</v>
+      </c>
+      <c r="H15" t="s" s="16">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1807,69 +2156,483 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.1719" style="17" customWidth="1"/>
-    <col min="2" max="2" width="14.1719" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.35156" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.67188" style="17" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.1719" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.6719" style="17" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="17" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="17" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="17" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="17" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="17" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="17" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="17" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="17" customWidth="1"/>
+    <col min="9" max="256" width="16.3516" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.65" customHeight="1">
+    <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="18">
+        <v>60</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" ht="28.65" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="18">
+      <c r="B2" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="18">
+      <c r="C2" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="18">
+      <c r="D2" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="18">
+      <c r="E2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="18">
+      <c r="F2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="18">
+      <c r="G2" t="s" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="19">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s" s="19">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s" s="19">
-        <v>46</v>
-      </c>
-      <c r="F2" s="20">
-        <v>23278101398</v>
-      </c>
-      <c r="G2" s="20">
+      <c r="H2" t="s" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="14.7" customHeight="1">
+      <c r="A3" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s" s="20">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s" s="20">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s" s="20">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s" s="20">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s" s="20">
+        <v>66</v>
+      </c>
+      <c r="G3" s="21">
+        <v>23279505128</v>
+      </c>
+      <c r="H3" t="s" s="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" t="s" s="20">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="20">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s" s="20">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s" s="20">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s" s="20">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s" s="20">
+        <v>72</v>
+      </c>
+      <c r="G4" s="21">
+        <v>23278102098</v>
+      </c>
+      <c r="H4" t="s" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" t="s" s="20">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="20">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s" s="20">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s" s="20">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s" s="20">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G5" t="s" s="20">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" t="s" s="20">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s" s="20">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s" s="20">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s" s="20">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s" s="20">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s" s="20">
+        <v>83</v>
+      </c>
+      <c r="G6" s="21">
+        <v>23278409544</v>
+      </c>
+      <c r="H6" t="s" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" t="s" s="20">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s" s="20">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s" s="20">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s" s="20">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s" s="20">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s" s="20">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s" s="20">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" t="s" s="24">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s" s="25">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s" s="25">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s" s="25">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s" s="25">
+        <v>16</v>
+      </c>
+      <c r="F8" s="26">
+        <v>23288559110</v>
+      </c>
+      <c r="G8" s="26">
+        <v>23278691307</v>
+      </c>
+      <c r="H8" t="s" s="27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" t="s" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="25">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s" s="25">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s" s="25">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s" s="25">
+        <v>95</v>
+      </c>
+      <c r="F9" s="26">
+        <v>23288141577</v>
+      </c>
+      <c r="G9" s="26">
+        <v>23279617405</v>
+      </c>
+      <c r="H9" t="s" s="27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" t="s" s="24">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s" s="25">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s" s="25">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s" s="25">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s" s="25">
+        <v>97</v>
+      </c>
+      <c r="F10" s="26">
+        <v>23230409350</v>
+      </c>
+      <c r="G10" s="26">
+        <v>23278409606</v>
+      </c>
+      <c r="H10" t="s" s="27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" t="s" s="24">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s" s="25">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s" s="25">
+        <v>99</v>
+      </c>
+      <c r="D11" t="s" s="25">
+        <v>100</v>
+      </c>
+      <c r="E11" t="s" s="25">
+        <v>101</v>
+      </c>
+      <c r="F11" s="26">
+        <v>23280727364</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" t="s" s="27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" ht="14.7" customHeight="1">
+      <c r="A12" t="s" s="24">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s" s="25">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s" s="25">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s" s="25">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s" s="25">
+        <v>105</v>
+      </c>
+      <c r="F12" s="26">
+        <v>23299999999</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" t="s" s="27">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1719" style="29" customWidth="1"/>
+    <col min="2" max="2" width="14.1719" style="29" customWidth="1"/>
+    <col min="3" max="3" width="9.35156" style="29" customWidth="1"/>
+    <col min="4" max="4" width="9.67188" style="29" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="29" customWidth="1"/>
+    <col min="6" max="6" width="12" style="29" customWidth="1"/>
+    <col min="7" max="7" width="20.6719" style="29" customWidth="1"/>
+    <col min="8" max="256" width="16.3516" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="13.7" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s" s="4">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>110</v>
+      </c>
+      <c r="F2" s="5">
         <v>23278101938</v>
       </c>
+      <c r="G2" s="5">
+        <v>23278101938</v>
+      </c>
+    </row>
+    <row r="3" ht="15.2" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>114</v>
+      </c>
+      <c r="F3" s="11">
+        <v>23276144814</v>
+      </c>
+      <c r="G3" s="11">
+        <v>23278969368</v>
+      </c>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>